<commit_message>
Dashboard of metrics for final predictions vs. results
</commit_message>
<xml_diff>
--- a/ratings-2023.xlsx
+++ b/ratings-2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/PycharmProjects/tvratings-ssac2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591976F5-6EAC-8949-BAAC-9AC92C060056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94B8164-291A-E149-B6B6-7DF900A5E003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3700" yWindow="13700" windowWidth="37240" windowHeight="10280" xr2:uid="{BBDA95F9-3552-704A-ADE2-3350C5179C3F}"/>
   </bookViews>
@@ -790,9 +790,9 @@
   <dimension ref="A1:AA33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="760" activePane="bottomLeft"/>
+      <pane ySplit="760" topLeftCell="A21" activePane="bottomLeft"/>
       <selection sqref="A1:AA1"/>
-      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -900,6 +900,9 @@
       <c r="E2" t="s">
         <v>97</v>
       </c>
+      <c r="F2">
+        <v>3560000</v>
+      </c>
       <c r="G2">
         <v>2023</v>
       </c>
@@ -982,6 +985,9 @@
       <c r="E3" t="s">
         <v>117</v>
       </c>
+      <c r="F3">
+        <v>582000</v>
+      </c>
       <c r="G3">
         <v>2023</v>
       </c>
@@ -1064,6 +1070,9 @@
       <c r="E4" t="s">
         <v>101</v>
       </c>
+      <c r="F4">
+        <v>466000</v>
+      </c>
       <c r="G4">
         <v>2023</v>
       </c>
@@ -1146,6 +1155,9 @@
       <c r="E5" t="s">
         <v>93</v>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
       <c r="G5">
         <v>2023</v>
       </c>
@@ -1228,6 +1240,9 @@
       <c r="E6" t="s">
         <v>43</v>
       </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
       <c r="G6">
         <v>2023</v>
       </c>
@@ -1310,6 +1325,9 @@
       <c r="E7" t="s">
         <v>22</v>
       </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
       <c r="G7">
         <v>2023</v>
       </c>
@@ -1392,6 +1410,9 @@
       <c r="E8" t="s">
         <v>48</v>
       </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
       <c r="G8">
         <v>2023</v>
       </c>
@@ -1474,6 +1495,9 @@
       <c r="E9" t="s">
         <v>68</v>
       </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
       <c r="G9">
         <v>2023</v>
       </c>
@@ -1556,6 +1580,9 @@
       <c r="E10" t="s">
         <v>111</v>
       </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
       <c r="G10">
         <v>2023</v>
       </c>
@@ -1638,6 +1665,9 @@
       <c r="E11" t="s">
         <v>79</v>
       </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
       <c r="G11">
         <v>2023</v>
       </c>
@@ -1720,6 +1750,9 @@
       <c r="E12" t="s">
         <v>86</v>
       </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
       <c r="G12">
         <v>2023</v>
       </c>
@@ -1802,6 +1835,9 @@
       <c r="E13" t="s">
         <v>46</v>
       </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
       <c r="G13">
         <v>2023</v>
       </c>
@@ -1884,6 +1920,9 @@
       <c r="E14" t="s">
         <v>94</v>
       </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
       <c r="G14">
         <v>2023</v>
       </c>
@@ -1966,6 +2005,9 @@
       <c r="E15" t="s">
         <v>25</v>
       </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
       <c r="G15">
         <v>2023</v>
       </c>
@@ -2048,6 +2090,9 @@
       <c r="E16" t="s">
         <v>26</v>
       </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
       <c r="G16">
         <v>2023</v>
       </c>
@@ -2130,6 +2175,9 @@
       <c r="E17" t="s">
         <v>102</v>
       </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
       <c r="G17">
         <v>2023</v>
       </c>
@@ -2212,6 +2260,9 @@
       <c r="E18" t="s">
         <v>120</v>
       </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
       <c r="G18">
         <v>2023</v>
       </c>
@@ -2294,6 +2345,9 @@
       <c r="E19" t="s">
         <v>88</v>
       </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
       <c r="G19">
         <v>2023</v>
       </c>
@@ -2376,6 +2430,9 @@
       <c r="E20" t="s">
         <v>117</v>
       </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
       <c r="G20">
         <v>2023</v>
       </c>
@@ -2458,6 +2515,9 @@
       <c r="E21" t="s">
         <v>89</v>
       </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
       <c r="G21">
         <v>2023</v>
       </c>
@@ -2540,6 +2600,9 @@
       <c r="E22" t="s">
         <v>98</v>
       </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
       <c r="G22">
         <v>2023</v>
       </c>
@@ -2622,6 +2685,9 @@
       <c r="E23" t="s">
         <v>40</v>
       </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
       <c r="G23">
         <v>2023</v>
       </c>
@@ -2704,6 +2770,9 @@
       <c r="E24" t="s">
         <v>36</v>
       </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
       <c r="G24">
         <v>2023</v>
       </c>
@@ -2786,6 +2855,9 @@
       <c r="E25" t="s">
         <v>99</v>
       </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
       <c r="G25">
         <v>2023</v>
       </c>
@@ -2868,6 +2940,9 @@
       <c r="E26" t="s">
         <v>73</v>
       </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
       <c r="G26">
         <v>2023</v>
       </c>
@@ -2950,6 +3025,9 @@
       <c r="E27" t="s">
         <v>107</v>
       </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
       <c r="G27">
         <v>2023</v>
       </c>
@@ -3032,6 +3110,9 @@
       <c r="E28" t="s">
         <v>121</v>
       </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
       <c r="G28">
         <v>2023</v>
       </c>
@@ -3114,6 +3195,9 @@
       <c r="E29" t="s">
         <v>90</v>
       </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
       <c r="G29">
         <v>2023</v>
       </c>
@@ -3196,6 +3280,9 @@
       <c r="E30" t="s">
         <v>28</v>
       </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
       <c r="G30">
         <v>2023</v>
       </c>
@@ -3278,6 +3365,9 @@
       <c r="E31" t="s">
         <v>39</v>
       </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
       <c r="G31">
         <v>2023</v>
       </c>
@@ -3360,6 +3450,9 @@
       <c r="E32" t="s">
         <v>81</v>
       </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
       <c r="G32">
         <v>2023</v>
       </c>
@@ -3441,6 +3534,9 @@
       </c>
       <c r="E33" t="s">
         <v>66</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
       </c>
       <c r="G33">
         <v>2023</v>

</xml_diff>